<commit_message>
updating issues and config
</commit_message>
<xml_diff>
--- a/code/RCMGUI_Issues.xlsx
+++ b/code/RCMGUI_Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frazibw1/Documents/RCM_Measurements/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63533A6E-6ADE-874D-8EA3-EF4B27E9F37A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7892021-2F1B-5241-B023-9BEF15AC538B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16700" xr2:uid="{803B860E-67BF-7649-8198-70C53CB3C689}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
   <si>
     <t>Issue #</t>
   </si>
@@ -181,6 +181,9 @@
   </si>
   <si>
     <t>Move Settings data logging to separate files for clarity</t>
+  </si>
+  <si>
+    <t>Have Calibration set the mode properly</t>
   </si>
 </sst>
 </file>
@@ -547,8 +550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019EAE55-1733-DF40-9D68-6F8D4E15BE5E}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="118" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1175,6 +1178,15 @@
       <c r="A44" s="2">
         <v>43</v>
       </c>
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44" s="1">
+        <v>43451</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="2">

</xml_diff>

<commit_message>
updates to config and Issues
</commit_message>
<xml_diff>
--- a/code/RCMGUI_Issues.xlsx
+++ b/code/RCMGUI_Issues.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/frazibw1/Documents/RCM_Measurements/code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B82F59CF-8DC6-7841-854C-BACDE99340C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667B210E-56B9-7346-8305-9658C15FCBEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16700" xr2:uid="{803B860E-67BF-7649-8198-70C53CB3C689}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="57">
   <si>
     <t>Issue #</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Trying to stop and delete the stepper motor timer caused the crash</t>
+  </si>
+  <si>
+    <t>Allow GUI to select the calibration file on the PNA</t>
   </si>
 </sst>
 </file>
@@ -559,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{019EAE55-1733-DF40-9D68-6F8D4E15BE5E}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="118" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="118" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1232,6 +1235,15 @@
       <c r="A47" s="2">
         <v>46</v>
       </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47" s="1">
+        <v>43451</v>
+      </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="2">

</xml_diff>